<commit_message>
Proyecto y Calificaciones Parcial 2
</commit_message>
<xml_diff>
--- a/Parcial1.xlsx
+++ b/Parcial1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Universidad_Panamerica\2026-1\Ecuaciones_Diferenciales_y_Metodos_Numericos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Universidad_Panamerica\2026-1\Ecuaciones_Diferenciales_y_Metodos_Numericos\Curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4662A34E-8D02-4EEF-94EC-A7720D7E5EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2809F41-098A-4531-87D3-01DEDB9BB1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4414" yWindow="1414" windowWidth="12266" windowHeight="8537" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43030" yWindow="2520" windowWidth="10630" windowHeight="8610" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarea1" sheetId="1" r:id="rId1"/>
@@ -285,10 +285,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -900,16 +900,16 @@
       <c r="C2" s="3">
         <v>263902</v>
       </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
         <v>0.7</v>
       </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
         <f>(D2+E2+F2)/3</f>
         <v>0.9</v>
       </c>
@@ -924,10 +924,10 @@
       <c r="C3" s="6">
         <v>269101</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -939,16 +939,16 @@
       <c r="C4" s="3">
         <v>267980</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0.7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <v>0.7</v>
       </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
         <f t="shared" ref="G4" si="0">(D4+E4+F4)/3</f>
         <v>0.79999999999999993</v>
       </c>
@@ -963,10 +963,10 @@
       <c r="C5" s="6">
         <v>240221</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -978,16 +978,16 @@
       <c r="C6" s="3">
         <v>269225</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
         <f t="shared" ref="G6" si="1">(D6+E6+F6)/3</f>
         <v>1</v>
       </c>
@@ -1002,10 +1002,10 @@
       <c r="C7" s="6">
         <v>266532</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -1017,16 +1017,16 @@
       <c r="C8" s="3">
         <v>267689</v>
       </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
         <v>0.7</v>
       </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
         <f t="shared" ref="G8" si="2">(D8+E8+F8)/3</f>
         <v>0.9</v>
       </c>
@@ -1041,10 +1041,10 @@
       <c r="C9" s="6">
         <v>234727</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -1056,16 +1056,16 @@
       <c r="C10" s="3">
         <v>261343</v>
       </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
         <v>0.7</v>
       </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
         <f t="shared" ref="G10" si="3">(D10+E10+F10)/3</f>
         <v>0.9</v>
       </c>
@@ -1080,13 +1080,21 @@
       <c r="C11" s="6">
         <v>269112</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
@@ -1099,14 +1107,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1118,7 +1118,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1156,16 +1159,16 @@
       <c r="C2" s="3">
         <v>263902</v>
       </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
         <f>(D2+E2+F2)/3</f>
         <v>1</v>
       </c>
@@ -1180,10 +1183,10 @@
       <c r="C3" s="6">
         <v>269101</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -1195,16 +1198,16 @@
       <c r="C4" s="3">
         <v>267980</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0.7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <v>0.7</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>0.7</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="8">
         <f t="shared" ref="G4" si="0">(D4+E4+F4)/3</f>
         <v>0.69999999999999984</v>
       </c>
@@ -1219,10 +1222,10 @@
       <c r="C5" s="6">
         <v>240221</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -1234,16 +1237,16 @@
       <c r="C6" s="3">
         <v>269225</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
         <v>0.7</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="8">
         <f t="shared" ref="G6" si="1">(D6+E6+F6)/3</f>
         <v>0.9</v>
       </c>
@@ -1258,10 +1261,10 @@
       <c r="C7" s="6">
         <v>266532</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -1273,16 +1276,16 @@
       <c r="C8" s="3">
         <v>267689</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.9</v>
       </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
         <f t="shared" ref="G8" si="2">(D8+E8+F8)/3</f>
         <v>0.96666666666666667</v>
       </c>
@@ -1297,10 +1300,10 @@
       <c r="C9" s="6">
         <v>234727</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -1312,16 +1315,16 @@
       <c r="C10" s="3">
         <v>261343</v>
       </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
         <v>0.9</v>
       </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
         <f t="shared" ref="G10" si="3">(D10+E10+F10)/3</f>
         <v>0.96666666666666667</v>
       </c>
@@ -1336,13 +1339,17 @@
       <c r="C11" s="6">
         <v>269112</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
@@ -1359,10 +1366,6 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1434,31 +1437,31 @@
       <c r="C2" s="3">
         <v>263902</v>
       </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <v>1</v>
-      </c>
-      <c r="L2" s="7">
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
         <f>(D2+E2+F2+G2+H2+I2+J2+K2)/7</f>
         <v>1.1428571428571428</v>
       </c>
@@ -1473,15 +1476,15 @@
       <c r="C3" s="6">
         <v>269101</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -1493,31 +1496,31 @@
       <c r="C4" s="3">
         <v>267980</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
         <v>0</v>
       </c>
-      <c r="J4" s="7">
-        <v>1</v>
-      </c>
-      <c r="K4" s="7">
-        <v>1</v>
-      </c>
-      <c r="L4" s="7">
+      <c r="J4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="8">
         <f t="shared" ref="L4" si="0">(D4+E4+F4+G4+H4+I4+J4+K4)/7</f>
         <v>1</v>
       </c>
@@ -1532,15 +1535,15 @@
       <c r="C5" s="6">
         <v>240221</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -1552,31 +1555,31 @@
       <c r="C6" s="3">
         <v>269225</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
         <v>0.9</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7">
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
-        <v>1</v>
-      </c>
-      <c r="L6" s="7">
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8">
         <f t="shared" ref="L6" si="1">(D6+E6+F6+G6+H6+I6+J6+K6)/7</f>
         <v>1.1285714285714286</v>
       </c>
@@ -1591,15 +1594,15 @@
       <c r="C7" s="6">
         <v>266532</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -1611,31 +1614,31 @@
       <c r="C8" s="3">
         <v>267689</v>
       </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
         <v>0.7</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="8">
         <v>0.7</v>
       </c>
-      <c r="J8" s="7">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="8">
         <v>0</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="8">
         <f t="shared" ref="L8" si="2">(D8+E8+F8+G8+H8+I8+J8+K8)/7</f>
         <v>0.91428571428571437</v>
       </c>
@@ -1650,15 +1653,15 @@
       <c r="C9" s="6">
         <v>234727</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -1670,29 +1673,29 @@
       <c r="C10" s="3">
         <v>261343</v>
       </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
-        <v>1</v>
-      </c>
-      <c r="H10" s="7">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
         <v>0.7</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="8">
         <v>0.7</v>
       </c>
-      <c r="J10" s="7">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7">
+      <c r="J10" s="8">
+        <v>1</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8">
         <f t="shared" ref="L10" si="3">(D10+E10+F10+G10+H10+I10+J10+K10)/7</f>
         <v>0.91428571428571437</v>
       </c>
@@ -1707,47 +1710,18 @@
       <c r="C11" s="6">
         <v>269112</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
@@ -1764,6 +1738,35 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>